<commit_message>
sample script, plot ylim
a sample script is created, a ylim is added to the result plot
</commit_message>
<xml_diff>
--- a/results/simulation_results.xlsx
+++ b/results/simulation_results.xlsx
@@ -461,7 +461,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45688.375</v>
+        <v>45689.375</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45688.38541666666</v>
+        <v>45689.38541666666</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45688.39583333334</v>
+        <v>45689.39583333334</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45688.40625</v>
+        <v>45689.40625</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45688.41666666666</v>
+        <v>45689.41666666666</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45688.42708333334</v>
+        <v>45689.42708333334</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45688.4375</v>
+        <v>45689.4375</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -559,590 +559,590 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45688.44791666666</v>
+        <v>45689.44791666666</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>13.66666666666667</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1.833333333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45688.45833333334</v>
+        <v>45689.45833333334</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45688.46875</v>
+        <v>45689.46875</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45688.47916666666</v>
+        <v>45689.47916666666</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45688.48958333334</v>
+        <v>45689.48958333334</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45688.5</v>
+        <v>45689.5</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45688.51041666666</v>
+        <v>45689.51041666666</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45688.52083333334</v>
+        <v>45689.52083333334</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45688.53125</v>
+        <v>45689.53125</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45688.54166666666</v>
+        <v>45689.54166666666</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45688.55208333334</v>
+        <v>45689.55208333334</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45688.5625</v>
+        <v>45689.5625</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45688.57291666666</v>
+        <v>45689.57291666666</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45688.58333333334</v>
+        <v>45689.58333333334</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45688.59375</v>
+        <v>45689.59375</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45688.60416666666</v>
+        <v>45689.60416666666</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45688.61458333334</v>
+        <v>45689.61458333334</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45688.625</v>
+        <v>45689.625</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45688.63541666666</v>
+        <v>45689.63541666666</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45688.64583333334</v>
+        <v>45689.64583333334</v>
       </c>
       <c r="B28" t="n">
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45688.65625</v>
+        <v>45689.65625</v>
       </c>
       <c r="B29" t="n">
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45688.66666666666</v>
+        <v>45689.66666666666</v>
       </c>
       <c r="B30" t="n">
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45688.67708333334</v>
+        <v>45689.67708333334</v>
       </c>
       <c r="B31" t="n">
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45688.6875</v>
+        <v>45689.6875</v>
       </c>
       <c r="B32" t="n">
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45688.69791666666</v>
+        <v>45689.69791666666</v>
       </c>
       <c r="B33" t="n">
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45688.70833333334</v>
+        <v>45689.70833333334</v>
       </c>
       <c r="B34" t="n">
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45688.71875</v>
+        <v>45689.71875</v>
       </c>
       <c r="B35" t="n">
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D35" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45688.72916666666</v>
+        <v>45689.72916666666</v>
       </c>
       <c r="B36" t="n">
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45688.73958333334</v>
+        <v>45689.73958333334</v>
       </c>
       <c r="B37" t="n">
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45688.75</v>
+        <v>45689.75</v>
       </c>
       <c r="B38" t="n">
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45688.76041666666</v>
+        <v>45689.76041666666</v>
       </c>
       <c r="B39" t="n">
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45688.77083333334</v>
+        <v>45689.77083333334</v>
       </c>
       <c r="B40" t="n">
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45688.78125</v>
+        <v>45689.78125</v>
       </c>
       <c r="B41" t="n">
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45688.79166666666</v>
+        <v>45689.79166666666</v>
       </c>
       <c r="B42" t="n">
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D42" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45688.80208333334</v>
+        <v>45689.80208333334</v>
       </c>
       <c r="B43" t="n">
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D43" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45688.8125</v>
+        <v>45689.8125</v>
       </c>
       <c r="B44" t="n">
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45688.82291666666</v>
+        <v>45689.82291666666</v>
       </c>
       <c r="B45" t="n">
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45688.83333333334</v>
+        <v>45689.83333333334</v>
       </c>
       <c r="B46" t="n">
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45688.84375</v>
+        <v>45689.84375</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D47" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45688.85416666666</v>
+        <v>45689.85416666666</v>
       </c>
       <c r="B48" t="n">
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D48" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45688.86458333334</v>
+        <v>45689.86458333334</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D49" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45688.875</v>
+        <v>45689.875</v>
       </c>
       <c r="B50" t="n">
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>10.73333333333333</v>
+        <v>18.80000000000001</v>
       </c>
       <c r="D50" t="n">
-        <v>0.3666666666666666</v>
+        <v>4.399999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>